<commit_message>
update to cheat sheet
</commit_message>
<xml_diff>
--- a/Stata.Cheat.Sheet.Tim.Essam.xlsx
+++ b/Stata.Cheat.Sheet.Tim.Essam.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Stata Cheat Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Reshaping &amp; Collapsing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="291">
   <si>
     <t>Stata Cheat Sheet</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Describe data in memory.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Correlations of variables.</t>
   </si>
   <si>
@@ -347,9 +345,6 @@
     <t>regexr(s, re)</t>
   </si>
   <si>
-    <t>String editing</t>
-  </si>
-  <si>
     <t>substr()</t>
   </si>
   <si>
@@ -368,9 +363,6 @@
     <t>sustitute text</t>
   </si>
   <si>
-    <t>strdup()</t>
-  </si>
-  <si>
     <t>strreverse()</t>
   </si>
   <si>
@@ -545,9 +537,6 @@
     <t>scalar list</t>
   </si>
   <si>
-    <t>display contents of macros</t>
-  </si>
-  <si>
     <t>Regression</t>
   </si>
   <si>
@@ -576,9 +565,6 @@
   </si>
   <si>
     <t>make regression tables</t>
-  </si>
-  <si>
-    <t>assert</t>
   </si>
   <si>
     <t>Loops</t>
@@ -820,12 +806,205 @@
   <si>
     <t>graph combine  boxprice histprice, row(2) scheme(2)</t>
   </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>gdp2014</t>
+  </si>
+  <si>
+    <t>gdp2015</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>stub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stub1 </t>
+  </si>
+  <si>
+    <t>stub2</t>
+  </si>
+  <si>
+    <t>reshape wide gdp, i(id) j(year)</t>
+  </si>
+  <si>
+    <t>reshape long</t>
+  </si>
+  <si>
+    <t>to convert from long to wide</t>
+  </si>
+  <si>
+    <t>to convert from side to long</t>
+  </si>
+  <si>
+    <t>wide</t>
+  </si>
+  <si>
+    <t>CPC</t>
+  </si>
+  <si>
+    <t>CPC2014</t>
+  </si>
+  <si>
+    <t>CPC2015</t>
+  </si>
+  <si>
+    <t>nsplit</t>
+  </si>
+  <si>
+    <t>splits a numeric value in n new variables based on digit patterns</t>
+  </si>
+  <si>
+    <t>Verify the truth of a claim</t>
+  </si>
+  <si>
+    <t>Duplicate observations</t>
+  </si>
+  <si>
+    <t>Tabulate missing values</t>
+  </si>
+  <si>
+    <t>Print a list of macros defined in current session</t>
+  </si>
+  <si>
+    <t>Drop selected macros</t>
+  </si>
+  <si>
+    <t>Loop over values</t>
+  </si>
+  <si>
+    <t>Loop over items</t>
+  </si>
+  <si>
+    <t>define a scalar called 'a' and store the value 3 in it</t>
+  </si>
+  <si>
+    <t>display the contents of scalar a</t>
+  </si>
+  <si>
+    <t>define a scala called s and store a string value in it</t>
+  </si>
+  <si>
+    <t>display the concents of scalar s</t>
+  </si>
+  <si>
+    <t>word(s, n)</t>
+  </si>
+  <si>
+    <t>returns the nth word in s</t>
+  </si>
+  <si>
+    <t>performs a match of a regular expression and evaluates to 1 if regular expression re is satisfied by the string s, otherwise returns 0</t>
+  </si>
+  <si>
+    <t>replaces the first substring within s1 that matches re with s2 and returns the resulting string.</t>
+  </si>
+  <si>
+    <t>returns subexpression n from a previous regexm() match, where 0 &lt; n &lt; 10</t>
+  </si>
+  <si>
+    <t>split()</t>
+  </si>
+  <si>
+    <t>split string variables into parts</t>
+  </si>
+  <si>
+    <t>itrims()</t>
+  </si>
+  <si>
+    <t>collapses consecutive internal blanks into one blank</t>
+  </si>
+  <si>
+    <t>use `display word("This is a string", 3)` to test what a function does</t>
+  </si>
+  <si>
+    <t>String functions</t>
+  </si>
+  <si>
+    <t>returns a string in reverse order</t>
+  </si>
+  <si>
+    <t>Displays a simple summary of data attributes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pect mpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Create or change contents of a variable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>enerate mpgSquared = mpg * mpg</t>
+    </r>
+  </si>
+  <si>
+    <t>assert rep78 != .</t>
+  </si>
+  <si>
+    <t>display scalars</t>
+  </si>
+  <si>
+    <t>drop scalars</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -866,8 +1045,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,8 +1067,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -889,22 +1082,158 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,6 +1249,101 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2903220" y="1386840"/>
+          <a:ext cx="2545080" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>to convert from long to wide</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>reshape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> wide gdp, i(id) j(year)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>to convert from wide to long</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>reshape long gdp@ CPC@, i(id) j(year)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1185,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1199,25 +1623,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,10 +1653,10 @@
       </c>
       <c r="C4" s="1"/>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1244,10 +1668,10 @@
       </c>
       <c r="C5" s="1"/>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,10 +1682,10 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,10 +1696,10 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1286,44 +1710,44 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
         <v>63</v>
-      </c>
-      <c r="F11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,297 +1757,312 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
-      </c>
-      <c r="F21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" t="s">
+        <v>286</v>
+      </c>
+      <c r="E27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" t="s">
         <v>146</v>
-      </c>
-      <c r="F26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>288</v>
+      </c>
+      <c r="B30" t="s">
+        <v>261</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="B31" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B32" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E34" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>189</v>
+      </c>
+      <c r="B38" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,15 +2072,15 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>221</v>
+      <c r="A42" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -1649,609 +2088,689 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="B43" t="s">
-        <v>30</v>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>285</v>
+      </c>
+      <c r="B44" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B52" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="B58" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="B59" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="B62" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="B63" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>166</v>
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B69" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B70" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="B73" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>173</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B85" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B99" t="s">
         <v>84</v>
-      </c>
-      <c r="B99" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B100" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>92</v>
+      </c>
+      <c r="B109" t="s">
         <v>93</v>
-      </c>
-      <c r="B109" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>94</v>
+      </c>
+      <c r="B110" t="s">
         <v>95</v>
-      </c>
-      <c r="B110" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>96</v>
+      </c>
+      <c r="B111" t="s">
         <v>97</v>
-      </c>
-      <c r="B111" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="B114" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B116" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="B117" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B118" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="B119" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>103</v>
+        <v>259</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>260</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>107</v>
+        <v>282</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" t="s">
         <v>108</v>
-      </c>
-      <c r="B124" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B125" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B126" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>109</v>
+        <v>279</v>
       </c>
       <c r="B127" t="s">
-        <v>113</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="B128" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="B129" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>277</v>
+      </c>
+      <c r="B131" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>272</v>
+      </c>
+      <c r="B132" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B135" t="s">
-        <v>232</v>
+      <c r="A133" t="s">
+        <v>102</v>
+      </c>
+      <c r="B133" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
-        <v>237</v>
+      <c r="A136" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>238</v>
+        <v>128</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>241</v>
+        <v>228</v>
+      </c>
+      <c r="B138" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>174</v>
+      <c r="A142" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>175</v>
+      <c r="A143" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>189</v>
-      </c>
-      <c r="B147" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>162</v>
-      </c>
-      <c r="B153" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>163</v>
-      </c>
-      <c r="B154" t="s">
-        <v>179</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>184</v>
+      </c>
+      <c r="B150" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>177</v>
+        <v>159</v>
+      </c>
+      <c r="B156" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B157" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>176</v>
+      </c>
+      <c r="B160" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>124</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2261,4 +2780,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="2" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="2" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>2014</v>
+      </c>
+      <c r="D4" s="21">
+        <v>8.2776995523542887</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19">
+        <v>1</v>
+      </c>
+      <c r="H4" s="21">
+        <v>8.2776995523542887</v>
+      </c>
+      <c r="I4" s="21">
+        <v>9.9866665996543382</v>
+      </c>
+      <c r="J4" s="20">
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="19">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20">
+        <v>2015</v>
+      </c>
+      <c r="D5" s="21">
+        <v>9.9866665996543382</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23">
+        <v>9.1017539346814313</v>
+      </c>
+      <c r="I5" s="23">
+        <v>4.051646941729782</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20">
+        <v>2014</v>
+      </c>
+      <c r="D6" s="21">
+        <v>9.1017539346814313</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2015</v>
+      </c>
+      <c r="D7" s="23">
+        <v>4.051646941729782</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>